<commit_message>
changed tutorial files to personal examples
</commit_message>
<xml_diff>
--- a/ventas2017soloserie.xlsx
+++ b/ventas2017soloserie.xlsx
@@ -12,20 +12,26 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7050"/>
   </bookViews>
   <sheets>
-    <sheet name="ventas2017" sheetId="1" r:id="rId1"/>
+    <sheet name="ventas2017soloserie" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>Campaña</t>
+  </si>
+  <si>
+    <t>Venta en Soles</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -33,16 +39,316 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -50,15 +356,204 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -336,108 +831,108 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>201709</v>
-      </c>
-      <c r="B1">
-        <v>3770100.1398031702</v>
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>201707</v>
+        <v>201609</v>
       </c>
       <c r="B2">
-        <v>4167591.4440681902</v>
+        <v>3754115.6430000002</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>201714</v>
+        <v>201610</v>
       </c>
       <c r="B3">
-        <v>4029177.8712073001</v>
+        <v>3605306.8309999998</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>201717</v>
+        <v>201611</v>
       </c>
       <c r="B4">
-        <v>4121266.71447122</v>
+        <v>3485719.5639999998</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>201705</v>
+        <v>201612</v>
       </c>
       <c r="B5">
-        <v>3489235.1951649399</v>
+        <v>3529235.6940000001</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>201712</v>
+        <v>201613</v>
       </c>
       <c r="B6">
-        <v>4024204.08597642</v>
+        <v>3706474.1710000001</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>201708</v>
+        <v>201614</v>
       </c>
       <c r="B7">
-        <v>3650176.0903380499</v>
+        <v>3779886.0860000001</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>201706</v>
+        <v>201615</v>
       </c>
       <c r="B8">
-        <v>3504004.7091928101</v>
+        <v>4038124.01</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>201715</v>
+        <v>201616</v>
       </c>
       <c r="B9">
-        <v>3987573.6117923302</v>
+        <v>3759566.7259999998</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>201703</v>
+        <v>201617</v>
       </c>
       <c r="B10">
-        <v>3133152.0404303102</v>
+        <v>4104212.3489999999</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>201710</v>
+        <v>201618</v>
       </c>
       <c r="B11">
-        <v>3833308.56157463</v>
+        <v>3904858.031</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>201713</v>
+        <v>201701</v>
       </c>
       <c r="B12">
-        <v>3838855.1130536199</v>
+        <v>3037780.4739999999</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -445,47 +940,151 @@
         <v>201702</v>
       </c>
       <c r="B13">
-        <v>3265607.2428737301</v>
+        <v>3288034.253</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>201711</v>
+        <v>201703</v>
       </c>
       <c r="B14">
-        <v>4158012.0304606599</v>
+        <v>3194577.79</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>201701</v>
+        <v>201704</v>
       </c>
       <c r="B15">
-        <v>2994616.1342724599</v>
+        <v>3244420.8990000002</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>201716</v>
+        <v>201705</v>
       </c>
       <c r="B16">
-        <v>4183237.3476555301</v>
+        <v>3446417.2349999999</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>201718</v>
+        <v>201706</v>
       </c>
       <c r="B17">
-        <v>4349255.00291848</v>
+        <v>3401707.159</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>201704</v>
+        <v>201707</v>
       </c>
       <c r="B18">
-        <v>3299681.4189089499</v>
+        <v>3949839.844</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>201708</v>
+      </c>
+      <c r="B19">
+        <v>3533020.45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>201709</v>
+      </c>
+      <c r="B20">
+        <v>3587834.88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>201710</v>
+      </c>
+      <c r="B21">
+        <v>3698958.7710000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>201711</v>
+      </c>
+      <c r="B22">
+        <v>3968946.77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>201712</v>
+      </c>
+      <c r="B23">
+        <v>3894021.4360000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>201713</v>
+      </c>
+      <c r="B24">
+        <v>3654349.2820000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>201714</v>
+      </c>
+      <c r="B25">
+        <v>3865883.2620000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>201715</v>
+      </c>
+      <c r="B26">
+        <v>3876430.5809999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>201716</v>
+      </c>
+      <c r="B27">
+        <v>4099300.5269999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>201717</v>
+      </c>
+      <c r="B28">
+        <v>4062445.0649999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>201718</v>
+      </c>
+      <c r="B29">
+        <v>4293296.6519999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>201801</v>
+      </c>
+      <c r="B30">
+        <v>3148095.9139999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>201802</v>
+      </c>
+      <c r="B31">
+        <v>3349614.8489999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>